<commit_message>
add read me  Changes in login authentication
</commit_message>
<xml_diff>
--- a/Data/words.xlsx
+++ b/Data/words.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Users" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -22,14 +22,12 @@
   <fonts count="3">
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -47,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -71,6 +69,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -80,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -88,11 +101,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -165,7 +181,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -208,71 +224,13 @@
     <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -280,7 +238,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -303,7 +261,7 @@
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -377,24 +335,13 @@
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -416,11 +363,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
+          <a:path path="circle"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -435,31 +380,28 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:path path="circle"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1674,11 +1616,168 @@
       </c>
     </row>
   </sheetData>
+  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" useFirstPageNumber="0" pageOrder="downThenOver" usePrinterDefaults="1" blackAndWhite="0" draft="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Italian</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>restare</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>to stay, remain</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>potere</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>to be able to</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>temere</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>to fear</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>avere</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>to have</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>restare</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>to stay, remain</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>potere</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>to be able to</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>temere</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>to fear</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1693,17 +1792,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Italian</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Username</t>
         </is>
@@ -1712,12 +1811,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>trovare</t>
+          <t>mangiare</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>to find</t>
+          <t>to eat</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1729,70 +1828,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>divertire</t>
+          <t>chiedere</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>to have fun</t>
+          <t>to ask, demand</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Italian</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>mangiare</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>to eat</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>test</t>
+          <t>smfasihaly</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1816,26 +1862,53 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Username</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Password</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>LastLogin</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>pbkdf2:sha256:260000$odUYGqKqHTj6tNzJ$d89a5b37f9c0b668e8c55f6cb96e22606c5e30b2b13b2c8bd35ad3c87f23735e</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-06-24 01:39:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>test</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>pbkdf2:sha256:260000$lw2LK28xF2y9ZjO1$7c0065091daa5db832bafe622fad90c159da844961958c54c4f119ba737e8687</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>pbkdf2:sha256:260000$fLlISUIViT9HjYlU$8887200da04ba942d08b49a03dd27aa5b01a176afe31e146db825735c9c03343</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-06-23 17:42:30</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change ui and update pagination bug
</commit_message>
<xml_diff>
--- a/Data/words.xlsx
+++ b/Data/words.xlsx
@@ -1666,7 +1666,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-06-24 05:08:31</t>
+          <t>2024-06-24 08:48:02</t>
         </is>
       </c>
     </row>
@@ -1698,7 +1698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1731,12 +1731,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sentire</t>
+          <t>cadere</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>to feel, sense, hear</t>
+          <t>to fall</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1746,19 +1746,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>English to Italian</t>
+          <t>Italian to English</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>passare</t>
+          <t>scendere</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>to pass</t>
+          <t>to go down</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1768,19 +1768,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>English to Italian</t>
+          <t>Italian to English</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>vestire</t>
+          <t>tenere</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>to dress</t>
+          <t>to keep</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1790,315 +1790,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>fare</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>to make, do</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>cominciare</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>to start</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>vendere</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>to sell</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>salire</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>to go up</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
           <t>Italian to English</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>decidere</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>to decide</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Italian to English</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ascoltare</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>to listen</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Italian to English</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>lavorare</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>to work</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Italian to English</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>cambiare</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>to change</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>ridere</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>to laugh</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>chiudere</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>to close</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>smfasihaly</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>rispondere</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>to answer</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>scrivere</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>to write</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>dire</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>to say</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>spegnere</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>to turn off</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>English to Italian</t>
         </is>
       </c>
     </row>
@@ -2113,7 +1805,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2281,6 +1973,94 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ridere</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>to laugh</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Italian to English</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>chiudere</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>to close</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Italian to English</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>imparare</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>to learn</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Italian to English</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>incontrare</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>to encounter</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>smfasihaly</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Italian to English</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>